<commit_message>
Finished C data, and created some data validation checks
</commit_message>
<xml_diff>
--- a/Datasheets/VF_W_Gearboxes.xlsx
+++ b/Datasheets/VF_W_Gearboxes.xlsx
@@ -387,7 +387,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -496,10 +496,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1094,7 +1090,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -1776,7 +1772,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -2507,7 +2503,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -3238,7 +3234,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -3916,7 +3912,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -4698,7 +4694,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -5480,7 +5476,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -6156,7 +6152,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -6938,7 +6934,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -7714,13 +7710,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -8367,9 +8363,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q14" s="27"/>
-    </row>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:M1"/>
@@ -8970,7 +9003,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -9752,7 +9785,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -10375,7 +10408,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -11045,13 +11078,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -11804,10 +11837,72 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="M16" s="27"/>
-      <c r="Q16" s="27"/>
-    </row>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:M1"/>
@@ -11837,7 +11932,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -12513,7 +12608,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -13242,7 +13337,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -13918,7 +14013,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -14382,7 +14477,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -15058,7 +15153,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -16411,7 +16506,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -17034,7 +17129,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -17710,7 +17805,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -18386,7 +18481,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -19003,13 +19098,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -19656,9 +19751,71 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G14" s="16"/>
-    </row>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:M1"/>
@@ -20312,7 +20469,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -21100,7 +21257,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -21776,7 +21933,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -22452,7 +22609,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>
@@ -23234,7 +23391,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="12.14"/>

</xml_diff>